<commit_message>
Gathered new results with fixed operators, ready to test NN parameters.
</commit_message>
<xml_diff>
--- a/Data Gathered and Results/Initial Results Variations Default Parameters/Results.xlsx
+++ b/Data Gathered and Results/Initial Results Variations Default Parameters/Results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\git\SET10107Coursework\Data\Initial Results Variations Default Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark\git\SET10107Coursework\Data Gathered and Results\Initial Results Variations Default Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="0" windowWidth="16065" windowHeight="11610"/>
+    <workbookView xWindow="9360" yWindow="0" windowWidth="16065" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Initial benchmark" sheetId="1" r:id="rId1"/>
@@ -686,8 +686,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22190836381672757"/>
-          <c:y val="2.4418879614867196E-2"/>
+          <c:x val="0.16769405730255768"/>
+          <c:y val="1.2073162867968352E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -722,9 +722,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -741,45 +740,29 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="narHorz">
-              <a:fgClr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="114300">
-                <a:schemeClr val="accent1"/>
-              </a:innerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Initial benchmark'!$B$33:$C$38</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Initial benchmark'!$B$33:$C$42</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Initial benchmark'!$B$33:$C$35,'Initial benchmark'!$B$37:$C$39,'Initial benchmark'!$B$41:$C$42)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Negative Inversion</c:v>
@@ -787,16 +770,16 @@
                   <c:pt idx="1">
                     <c:v>Uniform</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Roulette</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>Tournament 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>Single Point</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>Double Point</c:v>
                   </c:pt>
                 </c:lvl>
@@ -804,10 +787,10 @@
                   <c:pt idx="0">
                     <c:v>Mutation 0.2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Selection</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>Crosspoint</c:v>
                   </c:pt>
                 </c:lvl>
@@ -816,31 +799,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Initial benchmark'!$D$33:$D$38</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Initial benchmark'!$D$33:$D$42</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Initial benchmark'!$D$33:$D$35,'Initial benchmark'!$D$37:$D$39,'Initial benchmark'!$D$41:$D$42)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.38224257639911E-2</c:v>
+                  <c:v>5.5541044889306848E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1588730424586846E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.8914265265089194E-2</c:v>
+                  <c:v>1.6915469775438775E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6496890923488745E-2</c:v>
+                  <c:v>3.6835158485267902E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8550100031969747E-2</c:v>
+                  <c:v>3.5621356179477724E-2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.6861056156608199E-2</c:v>
+                <c:pt idx="6">
+                  <c:v>3.8019563972000375E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4436950692745244E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FE58-4EE1-AAA4-F67328A173A6}"/>
@@ -862,45 +853,29 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="narHorz">
-              <a:fgClr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="114300">
-                <a:schemeClr val="accent2"/>
-              </a:innerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Initial benchmark'!$B$33:$C$38</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Initial benchmark'!$B$33:$C$42</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Initial benchmark'!$B$33:$C$35,'Initial benchmark'!$B$37:$C$39,'Initial benchmark'!$B$41:$C$42)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Negative Inversion</c:v>
@@ -908,16 +883,16 @@
                   <c:pt idx="1">
                     <c:v>Uniform</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Roulette</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>Tournament 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>Single Point</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>Double Point</c:v>
                   </c:pt>
                 </c:lvl>
@@ -925,10 +900,10 @@
                   <c:pt idx="0">
                     <c:v>Mutation 0.2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Selection</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>Crosspoint</c:v>
                   </c:pt>
                 </c:lvl>
@@ -937,31 +912,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Initial benchmark'!$E$33:$E$38</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Initial benchmark'!$E$33:$E$42</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Initial benchmark'!$E$33:$E$35,'Initial benchmark'!$E$37:$E$39,'Initial benchmark'!$E$41:$E$42)</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.2173015987058477E-4</c:v>
+                  <c:v>3.1432020799665152E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.1873213387847451E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6732592178019526E-4</c:v>
+                  <c:v>2.3848658253277152E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7313637196886402E-4</c:v>
+                  <c:v>1.7654298876948601E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4608789981544978E-4</c:v>
+                  <c:v>1.6162587748044265E-4</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.943743939336095E-4</c:v>
+                <c:pt idx="6">
+                  <c:v>1.7982007995041757E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5834878629951109E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FE58-4EE1-AAA4-F67328A173A6}"/>
@@ -983,45 +966,29 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:pattFill prst="narHorz">
-              <a:fgClr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="20000"/>
-                  <a:lumOff val="80000"/>
-                </a:schemeClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:innerShdw blurRad="114300">
-                <a:schemeClr val="accent3"/>
-              </a:innerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Initial benchmark'!$B$33:$C$38</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Initial benchmark'!$B$33:$C$42</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Initial benchmark'!$B$33:$C$35,'Initial benchmark'!$B$37:$C$39,'Initial benchmark'!$B$41:$C$42)</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Negative Inversion</c:v>
@@ -1029,16 +996,16 @@
                   <c:pt idx="1">
                     <c:v>Uniform</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Roulette</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>Tournament 2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>Single Point</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>Double Point</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1046,10 +1013,10 @@
                   <c:pt idx="0">
                     <c:v>Mutation 0.2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>Selection</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>Crosspoint</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1058,31 +1025,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Initial benchmark'!$F$33:$F$38</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Initial benchmark'!$F$33:$F$42</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Initial benchmark'!$F$33:$F$35,'Initial benchmark'!$F$37:$F$39,'Initial benchmark'!$F$41:$F$42)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.18546313556063351</c:v>
+                  <c:v>0.16534798470990275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20071965183872825</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.18867057697009348</c:v>
+                  <c:v>6.6489880032925996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.19751221042926825</c:v>
+                  <c:v>0.11059203771379972</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19391353949722326</c:v>
+                  <c:v>0.12124582702902903</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.19226924790213851</c:v>
+                <c:pt idx="6">
+                  <c:v>0.11549096790116831</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.11634689684166044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FE58-4EE1-AAA4-F67328A173A6}"/>
@@ -1097,11 +1072,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="164"/>
-        <c:overlap val="-22"/>
+        <c:smooth val="0"/>
         <c:axId val="439987672"/>
         <c:axId val="439991608"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="439987672"/>
         <c:scaling>
@@ -1357,37 +1331,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1988,16 +1931,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19052</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2322,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>6.4189133012072103E-2</v>
+        <v>1.667436945343E-2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2356,7 +2299,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>5.3847967527007802E-2</v>
+        <v>5.0871301541559097E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2367,7 +2310,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>5.9761132232630701E-2</v>
+        <v>1.5750366028770699E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2378,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>5.7858828288646198E-2</v>
+        <v>6.4044596917311805E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2389,7 +2332,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>5.90237653628162E-2</v>
+        <v>1.74895464728008E-2</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -2401,7 +2344,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>5.0454233775965897E-2</v>
+        <v>5.3378538053897598E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2412,7 +2355,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>6.3380891090828395E-2</v>
+        <v>1.7747597146753599E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2423,7 +2366,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>5.3128673464344502E-2</v>
+        <v>5.38697430444589E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,7 +2377,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>2.9848991848499502E-4</v>
+        <v>2.7098397702646501E-5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2445,7 +2388,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="1">
-        <v>2.46444500585663E-4</v>
+        <v>3.0623119066970801E-4</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2456,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>3.2586571607757202E-4</v>
+        <v>2.78906186967925E-5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2467,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1">
-        <v>1.9850355197255099E-4</v>
+        <v>3.4495174800879702E-4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2478,7 +2421,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="1">
-        <v>2.8781199618825598E-4</v>
+        <v>1.62213267046807E-5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2489,7 +2432,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>2.42426454308128E-4</v>
+        <v>2.7508904592255499E-4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2500,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>3.6276090476307501E-4</v>
+        <v>2.4184289908988899E-5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2511,7 +2454,7 @@
         <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>1.99546132615997E-4</v>
+        <v>3.31008847385546E-4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2522,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.192457722608183</v>
+        <v>6.9429590669948305E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2533,7 +2476,7 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>0.18607531247899101</v>
+        <v>0.15213359464880499</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,7 +2487,7 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>0.19262232134914201</v>
+        <v>5.9638537792456599E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2555,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>0.18352695144405801</v>
+        <v>0.16116642774398901</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2566,7 +2509,7 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>0.21242579615641599</v>
+        <v>6.2035536428848903E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2577,7 +2520,7 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>0.18500659053924901</v>
+        <v>0.17875959968492999</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2588,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>0.20537276724117201</v>
+        <v>7.48558552404502E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2599,7 +2542,7 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>0.18724368778023601</v>
+        <v>0.16933231676188701</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2652,15 +2595,15 @@
       </c>
       <c r="D33">
         <f>AVERAGE(C2,C4,C6,C8)</f>
-        <v>5.38224257639911E-2</v>
+        <v>5.5541044889306848E-2</v>
       </c>
       <c r="E33" s="1">
         <f>AVERAGE(C10,C12,C14,C16)</f>
-        <v>2.2173015987058477E-4</v>
+        <v>3.1432020799665152E-4</v>
       </c>
       <c r="F33">
         <f>AVERAGE(C18,C20,C22,C24)</f>
-        <v>0.18546313556063351</v>
+        <v>0.16534798470990275</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -2669,89 +2612,101 @@
       </c>
       <c r="D34">
         <f>AVERAGE(C1,C3,C5,C7)</f>
-        <v>6.1588730424586846E-2</v>
+        <v>1.6915469775438775E-2</v>
       </c>
       <c r="E34" s="1">
         <f>AVERAGE(C9,C11,C13,C15)</f>
-        <v>3.1873213387847451E-4</v>
+        <v>2.3848658253277152E-5</v>
       </c>
       <c r="F34">
         <f>AVERAGE(C17,C19,C21,C23)</f>
-        <v>0.20071965183872825</v>
+        <v>6.6489880032925996E-2</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35">
-        <f>AVERAGE(C1,C2,C3,C4)</f>
-        <v>5.8914265265089194E-2</v>
-      </c>
-      <c r="E35" s="1">
-        <f>AVERAGE(C9,C10,C11,C12)</f>
-        <v>2.6732592178019526E-4</v>
-      </c>
-      <c r="F35">
-        <f>AVERAGE(C17,C18,C19,C20)</f>
-        <v>0.18867057697009348</v>
-      </c>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36">
-        <f>AVERAGE(C5,C6,C7,C8)</f>
-        <v>5.6496890923488745E-2</v>
-      </c>
-      <c r="E36" s="1">
-        <f>AVERAGE(C13,C14,C15,C16)</f>
-        <v>2.7313637196886402E-4</v>
-      </c>
-      <c r="F36">
-        <f>AVERAGE(C21,C22,C23,C24)</f>
-        <v>0.19751221042926825</v>
-      </c>
+      <c r="E36" s="1"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D37">
-        <f>AVERAGE(C1,C4,C5,C8)</f>
-        <v>5.8550100031969747E-2</v>
+        <f>AVERAGE(C1,C2,C3,C4)</f>
+        <v>3.6835158485267902E-2</v>
       </c>
       <c r="E37" s="1">
-        <f>AVERAGE(C9,C12,C13,C16)</f>
-        <v>2.4608789981544978E-4</v>
+        <f>AVERAGE(C9,C10,C11,C12)</f>
+        <v>1.7654298876948601E-4</v>
       </c>
       <c r="F37">
-        <f>AVERAGE(C17,C20,C21,C24)</f>
-        <v>0.19391353949722326</v>
+        <f>AVERAGE(C17,C18,C19,C20)</f>
+        <v>0.11059203771379972</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <f>AVERAGE(C5,C6,C7,C8)</f>
+        <v>3.5621356179477724E-2</v>
+      </c>
+      <c r="E38" s="1">
+        <f>AVERAGE(C13,C14,C15,C16)</f>
+        <v>1.6162587748044265E-4</v>
+      </c>
+      <c r="F38">
+        <f>AVERAGE(C21,C22,C23,C24)</f>
+        <v>0.12124582702902903</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41">
+        <f>AVERAGE(C1,C4,C5,C8)</f>
+        <v>3.8019563972000375E-2</v>
+      </c>
+      <c r="E41" s="1">
+        <f>AVERAGE(C9,C12,C13,C16)</f>
+        <v>1.7982007995041757E-4</v>
+      </c>
+      <c r="F41">
+        <f>AVERAGE(C17,C20,C21,C24)</f>
+        <v>0.11549096790116831</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>17</v>
       </c>
-      <c r="D38">
+      <c r="D42">
         <f>AVERAGE(C2,C3,C6,C7)</f>
-        <v>5.6861056156608199E-2</v>
-      </c>
-      <c r="E38" s="1">
+        <v>3.4436950692745244E-2</v>
+      </c>
+      <c r="E42" s="1">
         <f>AVERAGE(C10,C11,C14,C15)</f>
-        <v>2.943743939336095E-4</v>
-      </c>
-      <c r="F38">
+        <v>1.5834878629951109E-4</v>
+      </c>
+      <c r="F42">
         <f>AVERAGE(C18,C19,C22,C23)</f>
-        <v>0.19226924790213851</v>
+        <v>0.11634689684166044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>